<commit_message>
Fixed issue with /bestssellers href and added new Amazon Product Detail table view
</commit_message>
<xml_diff>
--- a/database/database_development.xlsx
+++ b/database/database_development.xlsx
@@ -208,10 +208,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="39.57"/>

</xml_diff>

<commit_message>
Temp fix: Moving to Firefox browser
</commit_message>
<xml_diff>
--- a/database/database_development.xlsx
+++ b/database/database_development.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Account</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t xml:space="preserve">B081D8XDCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Majestic Pure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G9-CLOG-DZRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B0176UQBJU </t>
   </si>
 </sst>
 </file>
@@ -208,10 +217,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="39.57"/>
@@ -281,12 +290,18 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>

</xml_diff>